<commit_message>
added some variables to AllP readme
also removed some blank rows in AllP
</commit_message>
<xml_diff>
--- a/Data sets/APA/APA.xlsx
+++ b/Data sets/APA/APA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EliseSchramkowski\Documents\GitHub\thesis\Data sets\APA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54DAEF3-AB0D-4BA3-8425-6B82649032E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6174A626-A541-459C-B28E-5164B113C2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5292" yWindow="8472" windowWidth="15120" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistical reporting errors al" sheetId="1" r:id="rId1"/>
@@ -9286,8 +9286,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AG525"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A426" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="W451" sqref="W451"/>
+    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="W260" sqref="W260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>